<commit_message>
Actualizado diagrama de gant
</commit_message>
<xml_diff>
--- a/Desarrollo/SGT/Gestión/Diagrama de gant.xlsx
+++ b/Desarrollo/SGT/Gestión/Diagrama de gant.xlsx
@@ -4,25 +4,17 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="75" windowWidth="20115" windowHeight="8265"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="28515" windowHeight="12600"/>
   </bookViews>
   <sheets>
     <sheet name="SGT" sheetId="1" r:id="rId1"/>
-    <sheet name="Gomez" sheetId="2" r:id="rId2"/>
-    <sheet name="Peralta" sheetId="5" r:id="rId3"/>
-    <sheet name="Rodriguez" sheetId="4" r:id="rId4"/>
-    <sheet name="Soldevilla" sheetId="3" r:id="rId5"/>
-    <sheet name="Tineo" sheetId="6" r:id="rId6"/>
-    <sheet name="VargasM" sheetId="7" r:id="rId7"/>
-    <sheet name="Vega" sheetId="8" r:id="rId8"/>
-    <sheet name="Yance" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="51">
   <si>
     <t>Lu</t>
   </si>
@@ -109,6 +101,72 @@
   </si>
   <si>
     <t>Aprobación del documento de negocio - BPMN</t>
+  </si>
+  <si>
+    <t>Backend</t>
+  </si>
+  <si>
+    <t>Definir estructura del proyecto</t>
+  </si>
+  <si>
+    <t>Definir el modelo de datos</t>
+  </si>
+  <si>
+    <t>Instalar librerías necesarias y configuración</t>
+  </si>
+  <si>
+    <t>Módulo de acceso</t>
+  </si>
+  <si>
+    <t>Módulo de tesis - CRUD</t>
+  </si>
+  <si>
+    <t>Módulo de tesis - Funcionalidad adicional</t>
+  </si>
+  <si>
+    <t>Módulo de novedades - CRUD</t>
+  </si>
+  <si>
+    <t>Módulo de novedades - Funcionalidad adicional</t>
+  </si>
+  <si>
+    <t>Módulo usuario general - Tesis favoritas</t>
+  </si>
+  <si>
+    <t>Módulo usuario general - Perfil</t>
+  </si>
+  <si>
+    <t>Despliegue del sistema</t>
+  </si>
+  <si>
+    <t>Frontend</t>
+  </si>
+  <si>
+    <t>Crear estructura de vistas</t>
+  </si>
+  <si>
+    <t>Definir vistas necesarias</t>
+  </si>
+  <si>
+    <t>Importar scripts necesarios</t>
+  </si>
+  <si>
+    <t>Pruebas</t>
+  </si>
+  <si>
+    <t>JP/WV/DY</t>
+  </si>
+  <si>
+    <t>DG/AR/SS/CT/JV</t>
+  </si>
+  <si>
+    <t>Cierre de proyecto</t>
+  </si>
+  <si>
+    <t>Subida a producción</t>
+  </si>
+  <si>
+    <t>Manual de usuario</t>
   </si>
 </sst>
 </file>
@@ -221,7 +279,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -237,22 +295,45 @@
       <alignment vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -556,20 +637,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BO15"/>
+  <dimension ref="A1:BU45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.140625" customWidth="1"/>
-    <col min="5" max="67" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" customWidth="1"/>
+    <col min="5" max="5" width="3.85546875" customWidth="1"/>
+    <col min="6" max="73" width="3.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:73" x14ac:dyDescent="0.25">
       <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
@@ -759,9 +841,27 @@
       <c r="BO1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:67" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="D2" s="12" t="s">
+      <c r="BP1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="BQ1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BR1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="BS1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="BT1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="BU1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:73" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="D2" s="8" t="s">
         <v>17</v>
       </c>
       <c r="E2" s="2" t="s">
@@ -953,360 +1053,921 @@
       <c r="BO2" s="5">
         <v>43793</v>
       </c>
-    </row>
-    <row r="3" spans="1:67" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="BP2" s="4">
+        <v>43794</v>
+      </c>
+      <c r="BQ2" s="4">
+        <v>43795</v>
+      </c>
+      <c r="BR2" s="4">
+        <v>43796</v>
+      </c>
+      <c r="BS2" s="4">
+        <v>43797</v>
+      </c>
+      <c r="BT2" s="4">
+        <v>43798</v>
+      </c>
+      <c r="BU2" s="5">
+        <v>43799</v>
+      </c>
+    </row>
+    <row r="3" spans="1:73" x14ac:dyDescent="0.25">
+      <c r="A3" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="7" t="s">
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
       <c r="M3" s="11"/>
       <c r="N3" s="11"/>
-    </row>
-    <row r="4" spans="1:67" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
+      <c r="O3" s="9"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="9"/>
+      <c r="S3" s="9"/>
+      <c r="T3" s="9"/>
+      <c r="U3" s="9"/>
+      <c r="V3" s="9"/>
+      <c r="W3" s="9"/>
+      <c r="X3" s="9"/>
+      <c r="Y3" s="9"/>
+      <c r="Z3" s="9"/>
+      <c r="AA3" s="9"/>
+      <c r="AB3" s="9"/>
+      <c r="AC3" s="9"/>
+      <c r="AD3" s="9"/>
+      <c r="AE3" s="9"/>
+      <c r="AF3" s="9"/>
+      <c r="AG3" s="9"/>
+      <c r="AH3" s="9"/>
+      <c r="AI3" s="9"/>
+      <c r="AJ3" s="9"/>
+      <c r="AK3" s="9"/>
+      <c r="AL3" s="9"/>
+      <c r="AM3" s="9"/>
+      <c r="AN3" s="9"/>
+      <c r="AO3" s="9"/>
+      <c r="AP3" s="9"/>
+      <c r="AQ3" s="9"/>
+      <c r="AR3" s="9"/>
+      <c r="AS3" s="9"/>
+      <c r="AT3" s="9"/>
+      <c r="AU3" s="9"/>
+      <c r="AV3" s="9"/>
+      <c r="AW3" s="9"/>
+      <c r="AX3" s="9"/>
+      <c r="AY3" s="9"/>
+      <c r="AZ3" s="9"/>
+      <c r="BA3" s="9"/>
+      <c r="BB3" s="9"/>
+      <c r="BC3" s="9"/>
+      <c r="BD3" s="9"/>
+      <c r="BE3" s="9"/>
+      <c r="BF3" s="9"/>
+      <c r="BG3" s="9"/>
+      <c r="BH3" s="9"/>
+      <c r="BI3" s="9"/>
+      <c r="BJ3" s="9"/>
+      <c r="BK3" s="9"/>
+      <c r="BL3" s="9"/>
+      <c r="BM3" s="9"/>
+      <c r="BN3" s="9"/>
+      <c r="BO3" s="9"/>
+    </row>
+    <row r="4" spans="1:73" x14ac:dyDescent="0.25">
+      <c r="A4" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="7" t="s">
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-    </row>
-    <row r="5" spans="1:67" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="9"/>
+      <c r="R4" s="9"/>
+      <c r="S4" s="9"/>
+      <c r="T4" s="9"/>
+      <c r="U4" s="9"/>
+      <c r="V4" s="9"/>
+      <c r="W4" s="9"/>
+      <c r="X4" s="9"/>
+      <c r="Y4" s="9"/>
+      <c r="Z4" s="9"/>
+      <c r="AA4" s="9"/>
+      <c r="AB4" s="9"/>
+      <c r="AC4" s="9"/>
+      <c r="AD4" s="9"/>
+      <c r="AE4" s="9"/>
+      <c r="AF4" s="9"/>
+      <c r="AG4" s="9"/>
+      <c r="AH4" s="9"/>
+      <c r="AI4" s="9"/>
+      <c r="AJ4" s="9"/>
+      <c r="AK4" s="9"/>
+      <c r="AL4" s="9"/>
+      <c r="AM4" s="9"/>
+      <c r="AN4" s="9"/>
+      <c r="AO4" s="9"/>
+      <c r="AP4" s="9"/>
+      <c r="AQ4" s="9"/>
+      <c r="AR4" s="9"/>
+      <c r="AS4" s="9"/>
+      <c r="AT4" s="9"/>
+      <c r="AU4" s="9"/>
+      <c r="AV4" s="9"/>
+      <c r="AW4" s="9"/>
+      <c r="AX4" s="9"/>
+      <c r="AY4" s="9"/>
+      <c r="AZ4" s="9"/>
+      <c r="BA4" s="9"/>
+      <c r="BB4" s="9"/>
+      <c r="BC4" s="9"/>
+      <c r="BD4" s="9"/>
+      <c r="BE4" s="9"/>
+      <c r="BF4" s="9"/>
+      <c r="BG4" s="9"/>
+      <c r="BH4" s="9"/>
+      <c r="BI4" s="9"/>
+      <c r="BJ4" s="9"/>
+      <c r="BK4" s="9"/>
+      <c r="BL4" s="9"/>
+      <c r="BM4" s="9"/>
+      <c r="BN4" s="9"/>
+      <c r="BO4" s="9"/>
+    </row>
+    <row r="5" spans="1:73" x14ac:dyDescent="0.25">
+      <c r="A5" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="D5" t="s">
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="10"/>
-      <c r="M5" s="9"/>
-      <c r="N5" s="9"/>
-    </row>
-    <row r="6" spans="1:67" x14ac:dyDescent="0.25">
-      <c r="A6" s="15"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="15"/>
-      <c r="N6" s="15"/>
-      <c r="O6" s="15"/>
-      <c r="P6" s="15"/>
-      <c r="Q6" s="15"/>
-      <c r="R6" s="15"/>
-      <c r="S6" s="15"/>
-      <c r="T6" s="15"/>
-      <c r="U6" s="15"/>
-      <c r="V6" s="15"/>
-      <c r="W6" s="15"/>
-      <c r="X6" s="15"/>
-      <c r="Y6" s="15"/>
-      <c r="Z6" s="15"/>
-      <c r="AA6" s="15"/>
-      <c r="AB6" s="15"/>
-      <c r="AC6" s="15"/>
-      <c r="AD6" s="15"/>
-      <c r="AE6" s="15"/>
-      <c r="AF6" s="15"/>
-      <c r="AG6" s="15"/>
-      <c r="AH6" s="15"/>
-      <c r="AI6" s="15"/>
-      <c r="AJ6" s="15"/>
-      <c r="AK6" s="15"/>
-      <c r="AL6" s="15"/>
-      <c r="AM6" s="15"/>
-      <c r="AN6" s="15"/>
-      <c r="AO6" s="15"/>
-      <c r="AP6" s="15"/>
-      <c r="AQ6" s="15"/>
-      <c r="AR6" s="15"/>
-      <c r="AS6" s="15"/>
-      <c r="AT6" s="15"/>
-      <c r="AU6" s="15"/>
-      <c r="AV6" s="15"/>
-      <c r="AW6" s="15"/>
-      <c r="AX6" s="15"/>
-      <c r="AY6" s="15"/>
-      <c r="AZ6" s="15"/>
-      <c r="BA6" s="15"/>
-      <c r="BB6" s="15"/>
-      <c r="BC6" s="15"/>
-      <c r="BD6" s="15"/>
-      <c r="BE6" s="15"/>
-      <c r="BF6" s="15"/>
-      <c r="BG6" s="15"/>
-      <c r="BH6" s="15"/>
-      <c r="BI6" s="15"/>
-      <c r="BJ6" s="15"/>
-      <c r="BK6" s="15"/>
-      <c r="BL6" s="15"/>
-      <c r="BM6" s="15"/>
-      <c r="BN6" s="15"/>
-      <c r="BO6" s="15"/>
-    </row>
-    <row r="7" spans="1:67" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+      <c r="E5" s="9"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="12"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="9"/>
+      <c r="R5" s="9"/>
+      <c r="S5" s="9"/>
+      <c r="T5" s="9"/>
+      <c r="U5" s="9"/>
+      <c r="V5" s="9"/>
+      <c r="W5" s="9"/>
+      <c r="X5" s="9"/>
+      <c r="Y5" s="9"/>
+      <c r="Z5" s="9"/>
+      <c r="AA5" s="9"/>
+      <c r="AB5" s="9"/>
+      <c r="AC5" s="9"/>
+      <c r="AD5" s="9"/>
+      <c r="AE5" s="9"/>
+      <c r="AF5" s="9"/>
+      <c r="AG5" s="9"/>
+      <c r="AH5" s="9"/>
+      <c r="AI5" s="9"/>
+      <c r="AJ5" s="9"/>
+      <c r="AK5" s="9"/>
+      <c r="AL5" s="9"/>
+      <c r="AM5" s="9"/>
+      <c r="AN5" s="9"/>
+      <c r="AO5" s="9"/>
+      <c r="AP5" s="9"/>
+      <c r="AQ5" s="9"/>
+      <c r="AR5" s="9"/>
+      <c r="AS5" s="9"/>
+      <c r="AT5" s="9"/>
+      <c r="AU5" s="9"/>
+      <c r="AV5" s="9"/>
+      <c r="AW5" s="9"/>
+      <c r="AX5" s="9"/>
+      <c r="AY5" s="9"/>
+      <c r="AZ5" s="9"/>
+      <c r="BA5" s="9"/>
+      <c r="BB5" s="9"/>
+      <c r="BC5" s="9"/>
+      <c r="BD5" s="9"/>
+      <c r="BE5" s="9"/>
+      <c r="BF5" s="9"/>
+      <c r="BG5" s="9"/>
+      <c r="BH5" s="9"/>
+      <c r="BI5" s="9"/>
+      <c r="BJ5" s="9"/>
+      <c r="BK5" s="9"/>
+      <c r="BL5" s="9"/>
+      <c r="BM5" s="9"/>
+      <c r="BN5" s="9"/>
+      <c r="BO5" s="9"/>
+    </row>
+    <row r="6" spans="1:73" x14ac:dyDescent="0.25">
+      <c r="A6" s="20"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="20"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="20"/>
+      <c r="O6" s="20"/>
+      <c r="P6" s="20"/>
+      <c r="Q6" s="20"/>
+      <c r="R6" s="20"/>
+      <c r="S6" s="20"/>
+      <c r="T6" s="20"/>
+      <c r="U6" s="20"/>
+      <c r="V6" s="20"/>
+      <c r="W6" s="20"/>
+      <c r="X6" s="20"/>
+      <c r="Y6" s="20"/>
+      <c r="Z6" s="20"/>
+      <c r="AA6" s="20"/>
+      <c r="AB6" s="20"/>
+      <c r="AC6" s="20"/>
+      <c r="AD6" s="20"/>
+      <c r="AE6" s="20"/>
+      <c r="AF6" s="20"/>
+      <c r="AG6" s="20"/>
+      <c r="AH6" s="20"/>
+      <c r="AI6" s="20"/>
+      <c r="AJ6" s="20"/>
+      <c r="AK6" s="20"/>
+      <c r="AL6" s="20"/>
+      <c r="AM6" s="20"/>
+      <c r="AN6" s="20"/>
+      <c r="AO6" s="20"/>
+      <c r="AP6" s="20"/>
+      <c r="AQ6" s="20"/>
+      <c r="AR6" s="20"/>
+      <c r="AS6" s="20"/>
+      <c r="AT6" s="20"/>
+      <c r="AU6" s="20"/>
+      <c r="AV6" s="20"/>
+      <c r="AW6" s="20"/>
+      <c r="AX6" s="20"/>
+      <c r="AY6" s="20"/>
+      <c r="AZ6" s="20"/>
+      <c r="BA6" s="20"/>
+      <c r="BB6" s="20"/>
+      <c r="BC6" s="20"/>
+      <c r="BD6" s="20"/>
+      <c r="BE6" s="20"/>
+      <c r="BF6" s="20"/>
+      <c r="BG6" s="20"/>
+      <c r="BH6" s="20"/>
+      <c r="BI6" s="20"/>
+      <c r="BJ6" s="20"/>
+      <c r="BK6" s="20"/>
+      <c r="BL6" s="20"/>
+      <c r="BM6" s="20"/>
+      <c r="BN6" s="20"/>
+      <c r="BO6" s="20"/>
+    </row>
+    <row r="7" spans="1:73" x14ac:dyDescent="0.25">
+      <c r="A7" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
       <c r="I7" s="11"/>
-    </row>
-    <row r="8" spans="1:67" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="9"/>
+      <c r="R7" s="9"/>
+      <c r="S7" s="9"/>
+      <c r="T7" s="9"/>
+      <c r="U7" s="9"/>
+      <c r="V7" s="9"/>
+      <c r="W7" s="9"/>
+      <c r="X7" s="9"/>
+      <c r="Y7" s="9"/>
+      <c r="Z7" s="9"/>
+      <c r="AA7" s="9"/>
+      <c r="AB7" s="9"/>
+      <c r="AC7" s="9"/>
+      <c r="AD7" s="9"/>
+      <c r="AE7" s="9"/>
+      <c r="AF7" s="9"/>
+      <c r="AG7" s="9"/>
+      <c r="AH7" s="9"/>
+      <c r="AI7" s="9"/>
+      <c r="AJ7" s="9"/>
+      <c r="AK7" s="9"/>
+      <c r="AL7" s="9"/>
+      <c r="AM7" s="9"/>
+      <c r="AN7" s="9"/>
+      <c r="AO7" s="9"/>
+      <c r="AP7" s="9"/>
+      <c r="AQ7" s="9"/>
+      <c r="AR7" s="9"/>
+      <c r="AS7" s="9"/>
+      <c r="AT7" s="9"/>
+      <c r="AU7" s="9"/>
+      <c r="AV7" s="9"/>
+      <c r="AW7" s="9"/>
+      <c r="AX7" s="9"/>
+      <c r="AY7" s="9"/>
+      <c r="AZ7" s="9"/>
+      <c r="BA7" s="9"/>
+      <c r="BB7" s="9"/>
+      <c r="BC7" s="9"/>
+      <c r="BD7" s="9"/>
+      <c r="BE7" s="9"/>
+      <c r="BF7" s="9"/>
+      <c r="BG7" s="9"/>
+      <c r="BH7" s="9"/>
+      <c r="BI7" s="9"/>
+      <c r="BJ7" s="9"/>
+      <c r="BK7" s="9"/>
+      <c r="BL7" s="9"/>
+      <c r="BM7" s="9"/>
+      <c r="BN7" s="9"/>
+      <c r="BO7" s="9"/>
+    </row>
+    <row r="8" spans="1:73" x14ac:dyDescent="0.25">
+      <c r="A8" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" t="s">
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-    </row>
-    <row r="9" spans="1:67" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="9"/>
+      <c r="S8" s="9"/>
+      <c r="T8" s="9"/>
+      <c r="U8" s="9"/>
+      <c r="V8" s="9"/>
+      <c r="W8" s="9"/>
+      <c r="X8" s="9"/>
+      <c r="Y8" s="9"/>
+      <c r="Z8" s="9"/>
+      <c r="AA8" s="9"/>
+      <c r="AB8" s="9"/>
+      <c r="AC8" s="9"/>
+      <c r="AD8" s="9"/>
+      <c r="AE8" s="9"/>
+      <c r="AF8" s="9"/>
+      <c r="AG8" s="9"/>
+      <c r="AH8" s="9"/>
+      <c r="AI8" s="9"/>
+      <c r="AJ8" s="9"/>
+      <c r="AK8" s="9"/>
+      <c r="AL8" s="9"/>
+      <c r="AM8" s="9"/>
+      <c r="AN8" s="9"/>
+      <c r="AO8" s="9"/>
+      <c r="AP8" s="9"/>
+      <c r="AQ8" s="9"/>
+      <c r="AR8" s="9"/>
+      <c r="AS8" s="9"/>
+      <c r="AT8" s="9"/>
+      <c r="AU8" s="9"/>
+      <c r="AV8" s="9"/>
+      <c r="AW8" s="9"/>
+      <c r="AX8" s="9"/>
+      <c r="AY8" s="9"/>
+      <c r="AZ8" s="9"/>
+      <c r="BA8" s="9"/>
+      <c r="BB8" s="9"/>
+      <c r="BC8" s="9"/>
+      <c r="BD8" s="9"/>
+      <c r="BE8" s="9"/>
+      <c r="BF8" s="9"/>
+      <c r="BG8" s="9"/>
+      <c r="BH8" s="9"/>
+      <c r="BI8" s="9"/>
+      <c r="BJ8" s="9"/>
+      <c r="BK8" s="9"/>
+      <c r="BL8" s="9"/>
+      <c r="BM8" s="9"/>
+      <c r="BN8" s="9"/>
+      <c r="BO8" s="9"/>
+    </row>
+    <row r="9" spans="1:73" x14ac:dyDescent="0.25">
+      <c r="A9" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="7" t="s">
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="G9" s="10"/>
-      <c r="I9" s="9"/>
-    </row>
-    <row r="10" spans="1:67" x14ac:dyDescent="0.25">
-      <c r="A10" s="15"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="15"/>
-      <c r="M10" s="15"/>
-      <c r="N10" s="15"/>
-      <c r="O10" s="15"/>
-      <c r="P10" s="15"/>
-      <c r="Q10" s="15"/>
-      <c r="R10" s="15"/>
-      <c r="S10" s="15"/>
-      <c r="T10" s="15"/>
-      <c r="U10" s="15"/>
-      <c r="V10" s="15"/>
-      <c r="W10" s="15"/>
-      <c r="X10" s="15"/>
-      <c r="Y10" s="15"/>
-      <c r="Z10" s="15"/>
-      <c r="AA10" s="15"/>
-      <c r="AB10" s="15"/>
-      <c r="AC10" s="15"/>
-      <c r="AD10" s="15"/>
-      <c r="AE10" s="15"/>
-      <c r="AF10" s="15"/>
-      <c r="AG10" s="15"/>
-      <c r="AH10" s="15"/>
-      <c r="AI10" s="15"/>
-      <c r="AJ10" s="15"/>
-      <c r="AK10" s="15"/>
-      <c r="AL10" s="15"/>
-      <c r="AM10" s="15"/>
-      <c r="AN10" s="15"/>
-      <c r="AO10" s="15"/>
-      <c r="AP10" s="15"/>
-      <c r="AQ10" s="15"/>
-      <c r="AR10" s="15"/>
-      <c r="AS10" s="15"/>
-      <c r="AT10" s="15"/>
-      <c r="AU10" s="15"/>
-      <c r="AV10" s="15"/>
-      <c r="AW10" s="15"/>
-      <c r="AX10" s="15"/>
-      <c r="AY10" s="15"/>
-      <c r="AZ10" s="15"/>
-      <c r="BA10" s="15"/>
-      <c r="BB10" s="15"/>
-      <c r="BC10" s="15"/>
-      <c r="BD10" s="15"/>
-      <c r="BE10" s="15"/>
-      <c r="BF10" s="15"/>
-      <c r="BG10" s="15"/>
-      <c r="BH10" s="15"/>
-      <c r="BI10" s="15"/>
-      <c r="BJ10" s="15"/>
-      <c r="BK10" s="15"/>
-      <c r="BL10" s="15"/>
-      <c r="BM10" s="15"/>
-      <c r="BN10" s="15"/>
-      <c r="BO10" s="15"/>
-    </row>
-    <row r="11" spans="1:67" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="9"/>
+      <c r="S9" s="9"/>
+      <c r="T9" s="9"/>
+      <c r="U9" s="9"/>
+      <c r="V9" s="9"/>
+      <c r="W9" s="9"/>
+      <c r="X9" s="9"/>
+      <c r="Y9" s="9"/>
+      <c r="Z9" s="9"/>
+      <c r="AA9" s="9"/>
+      <c r="AB9" s="9"/>
+      <c r="AC9" s="9"/>
+      <c r="AD9" s="9"/>
+      <c r="AE9" s="9"/>
+      <c r="AF9" s="9"/>
+      <c r="AG9" s="9"/>
+      <c r="AH9" s="9"/>
+      <c r="AI9" s="9"/>
+      <c r="AJ9" s="9"/>
+      <c r="AK9" s="9"/>
+      <c r="AL9" s="9"/>
+      <c r="AM9" s="9"/>
+      <c r="AN9" s="9"/>
+      <c r="AO9" s="9"/>
+      <c r="AP9" s="9"/>
+      <c r="AQ9" s="9"/>
+      <c r="AR9" s="9"/>
+      <c r="AS9" s="9"/>
+      <c r="AT9" s="9"/>
+      <c r="AU9" s="9"/>
+      <c r="AV9" s="9"/>
+      <c r="AW9" s="9"/>
+      <c r="AX9" s="9"/>
+      <c r="AY9" s="9"/>
+      <c r="AZ9" s="9"/>
+      <c r="BA9" s="9"/>
+      <c r="BB9" s="9"/>
+      <c r="BC9" s="9"/>
+      <c r="BD9" s="9"/>
+      <c r="BE9" s="9"/>
+      <c r="BF9" s="9"/>
+      <c r="BG9" s="9"/>
+      <c r="BH9" s="9"/>
+      <c r="BI9" s="9"/>
+      <c r="BJ9" s="9"/>
+      <c r="BK9" s="9"/>
+      <c r="BL9" s="9"/>
+      <c r="BM9" s="9"/>
+      <c r="BN9" s="9"/>
+      <c r="BO9" s="9"/>
+    </row>
+    <row r="10" spans="1:73" x14ac:dyDescent="0.25">
+      <c r="A10" s="20"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="20"/>
+      <c r="N10" s="20"/>
+      <c r="O10" s="20"/>
+      <c r="P10" s="20"/>
+      <c r="Q10" s="20"/>
+      <c r="R10" s="20"/>
+      <c r="S10" s="20"/>
+      <c r="T10" s="20"/>
+      <c r="U10" s="20"/>
+      <c r="V10" s="20"/>
+      <c r="W10" s="20"/>
+      <c r="X10" s="20"/>
+      <c r="Y10" s="20"/>
+      <c r="Z10" s="20"/>
+      <c r="AA10" s="20"/>
+      <c r="AB10" s="20"/>
+      <c r="AC10" s="20"/>
+      <c r="AD10" s="20"/>
+      <c r="AE10" s="20"/>
+      <c r="AF10" s="20"/>
+      <c r="AG10" s="20"/>
+      <c r="AH10" s="20"/>
+      <c r="AI10" s="20"/>
+      <c r="AJ10" s="20"/>
+      <c r="AK10" s="20"/>
+      <c r="AL10" s="20"/>
+      <c r="AM10" s="20"/>
+      <c r="AN10" s="20"/>
+      <c r="AO10" s="20"/>
+      <c r="AP10" s="20"/>
+      <c r="AQ10" s="20"/>
+      <c r="AR10" s="20"/>
+      <c r="AS10" s="20"/>
+      <c r="AT10" s="20"/>
+      <c r="AU10" s="20"/>
+      <c r="AV10" s="20"/>
+      <c r="AW10" s="20"/>
+      <c r="AX10" s="20"/>
+      <c r="AY10" s="20"/>
+      <c r="AZ10" s="20"/>
+      <c r="BA10" s="20"/>
+      <c r="BB10" s="20"/>
+      <c r="BC10" s="20"/>
+      <c r="BD10" s="20"/>
+      <c r="BE10" s="20"/>
+      <c r="BF10" s="20"/>
+      <c r="BG10" s="20"/>
+      <c r="BH10" s="20"/>
+      <c r="BI10" s="20"/>
+      <c r="BJ10" s="20"/>
+      <c r="BK10" s="20"/>
+      <c r="BL10" s="20"/>
+      <c r="BM10" s="20"/>
+      <c r="BN10" s="20"/>
+      <c r="BO10" s="20"/>
+    </row>
+    <row r="11" spans="1:73" x14ac:dyDescent="0.25">
+      <c r="A11" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="I11" s="10"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="13"/>
       <c r="J11" s="11"/>
       <c r="K11" s="11"/>
       <c r="L11" s="11"/>
-    </row>
-    <row r="12" spans="1:67" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="9"/>
+      <c r="R11" s="9"/>
+      <c r="S11" s="9"/>
+      <c r="T11" s="9"/>
+      <c r="U11" s="9"/>
+      <c r="V11" s="9"/>
+      <c r="W11" s="9"/>
+      <c r="X11" s="9"/>
+      <c r="Y11" s="9"/>
+      <c r="Z11" s="9"/>
+      <c r="AA11" s="9"/>
+      <c r="AB11" s="9"/>
+      <c r="AC11" s="9"/>
+      <c r="AD11" s="9"/>
+      <c r="AE11" s="9"/>
+      <c r="AF11" s="9"/>
+      <c r="AG11" s="9"/>
+      <c r="AH11" s="9"/>
+      <c r="AI11" s="9"/>
+      <c r="AJ11" s="9"/>
+      <c r="AK11" s="9"/>
+      <c r="AL11" s="9"/>
+      <c r="AM11" s="9"/>
+      <c r="AN11" s="9"/>
+      <c r="AO11" s="9"/>
+      <c r="AP11" s="9"/>
+      <c r="AQ11" s="9"/>
+      <c r="AR11" s="9"/>
+      <c r="AS11" s="9"/>
+      <c r="AT11" s="9"/>
+      <c r="AU11" s="9"/>
+      <c r="AV11" s="9"/>
+      <c r="AW11" s="9"/>
+      <c r="AX11" s="9"/>
+      <c r="AY11" s="9"/>
+      <c r="AZ11" s="9"/>
+      <c r="BA11" s="9"/>
+      <c r="BB11" s="9"/>
+      <c r="BC11" s="9"/>
+      <c r="BD11" s="9"/>
+      <c r="BE11" s="9"/>
+      <c r="BF11" s="9"/>
+      <c r="BG11" s="9"/>
+      <c r="BH11" s="9"/>
+      <c r="BI11" s="9"/>
+      <c r="BJ11" s="9"/>
+      <c r="BK11" s="9"/>
+      <c r="BL11" s="9"/>
+      <c r="BM11" s="9"/>
+      <c r="BN11" s="9"/>
+      <c r="BO11" s="9"/>
+    </row>
+    <row r="12" spans="1:73" x14ac:dyDescent="0.25">
+      <c r="A12" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" t="s">
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="I12" s="10"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9"/>
-    </row>
-    <row r="13" spans="1:67" x14ac:dyDescent="0.25">
-      <c r="A13" s="15" t="s">
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="9"/>
+      <c r="R12" s="9"/>
+      <c r="S12" s="9"/>
+      <c r="T12" s="9"/>
+      <c r="U12" s="9"/>
+      <c r="V12" s="9"/>
+      <c r="W12" s="9"/>
+      <c r="X12" s="9"/>
+      <c r="Y12" s="9"/>
+      <c r="Z12" s="9"/>
+      <c r="AA12" s="9"/>
+      <c r="AB12" s="9"/>
+      <c r="AC12" s="9"/>
+      <c r="AD12" s="9"/>
+      <c r="AE12" s="9"/>
+      <c r="AF12" s="9"/>
+      <c r="AG12" s="9"/>
+      <c r="AH12" s="9"/>
+      <c r="AI12" s="9"/>
+      <c r="AJ12" s="9"/>
+      <c r="AK12" s="9"/>
+      <c r="AL12" s="9"/>
+      <c r="AM12" s="9"/>
+      <c r="AN12" s="9"/>
+      <c r="AO12" s="9"/>
+      <c r="AP12" s="9"/>
+      <c r="AQ12" s="9"/>
+      <c r="AR12" s="9"/>
+      <c r="AS12" s="9"/>
+      <c r="AT12" s="9"/>
+      <c r="AU12" s="9"/>
+      <c r="AV12" s="9"/>
+      <c r="AW12" s="9"/>
+      <c r="AX12" s="9"/>
+      <c r="AY12" s="9"/>
+      <c r="AZ12" s="9"/>
+      <c r="BA12" s="9"/>
+      <c r="BB12" s="9"/>
+      <c r="BC12" s="9"/>
+      <c r="BD12" s="9"/>
+      <c r="BE12" s="9"/>
+      <c r="BF12" s="9"/>
+      <c r="BG12" s="9"/>
+      <c r="BH12" s="9"/>
+      <c r="BI12" s="9"/>
+      <c r="BJ12" s="9"/>
+      <c r="BK12" s="9"/>
+      <c r="BL12" s="9"/>
+      <c r="BM12" s="9"/>
+      <c r="BN12" s="9"/>
+      <c r="BO12" s="9"/>
+    </row>
+    <row r="13" spans="1:73" x14ac:dyDescent="0.25">
+      <c r="A13" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="7" t="s">
+      <c r="B13" s="20"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="L13" s="9"/>
-    </row>
-    <row r="14" spans="1:67" x14ac:dyDescent="0.25">
-      <c r="A14" s="15"/>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="15"/>
-      <c r="L14" s="15"/>
-      <c r="M14" s="15"/>
-      <c r="N14" s="15"/>
-      <c r="O14" s="15"/>
-      <c r="P14" s="15"/>
-      <c r="Q14" s="15"/>
-      <c r="R14" s="15"/>
-      <c r="S14" s="15"/>
-      <c r="T14" s="15"/>
-      <c r="U14" s="15"/>
-      <c r="V14" s="15"/>
-      <c r="W14" s="15"/>
-      <c r="X14" s="15"/>
-      <c r="Y14" s="15"/>
-      <c r="Z14" s="15"/>
-      <c r="AA14" s="15"/>
-      <c r="AB14" s="15"/>
-      <c r="AC14" s="15"/>
-      <c r="AD14" s="15"/>
-      <c r="AE14" s="15"/>
-      <c r="AF14" s="15"/>
-      <c r="AG14" s="15"/>
-      <c r="AH14" s="15"/>
-      <c r="AI14" s="15"/>
-      <c r="AJ14" s="15"/>
-      <c r="AK14" s="15"/>
-      <c r="AL14" s="15"/>
-      <c r="AM14" s="15"/>
-      <c r="AN14" s="15"/>
-      <c r="AO14" s="15"/>
-      <c r="AP14" s="15"/>
-      <c r="AQ14" s="15"/>
-      <c r="AR14" s="15"/>
-      <c r="AS14" s="15"/>
-      <c r="AT14" s="15"/>
-      <c r="AU14" s="15"/>
-      <c r="AV14" s="15"/>
-      <c r="AW14" s="15"/>
-      <c r="AX14" s="15"/>
-      <c r="AY14" s="15"/>
-      <c r="AZ14" s="15"/>
-      <c r="BA14" s="15"/>
-      <c r="BB14" s="15"/>
-      <c r="BC14" s="15"/>
-      <c r="BD14" s="15"/>
-      <c r="BE14" s="15"/>
-      <c r="BF14" s="15"/>
-      <c r="BG14" s="15"/>
-      <c r="BH14" s="15"/>
-      <c r="BI14" s="15"/>
-      <c r="BJ14" s="15"/>
-      <c r="BK14" s="15"/>
-      <c r="BL14" s="15"/>
-      <c r="BM14" s="15"/>
-      <c r="BN14" s="15"/>
-      <c r="BO14" s="15"/>
-    </row>
-    <row r="15" spans="1:67" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="9"/>
+      <c r="R13" s="9"/>
+      <c r="S13" s="9"/>
+      <c r="T13" s="9"/>
+      <c r="U13" s="9"/>
+      <c r="V13" s="9"/>
+      <c r="W13" s="9"/>
+      <c r="X13" s="9"/>
+      <c r="Y13" s="9"/>
+      <c r="Z13" s="9"/>
+      <c r="AA13" s="9"/>
+      <c r="AB13" s="9"/>
+      <c r="AC13" s="9"/>
+      <c r="AD13" s="9"/>
+      <c r="AE13" s="9"/>
+      <c r="AF13" s="9"/>
+      <c r="AG13" s="9"/>
+      <c r="AH13" s="9"/>
+      <c r="AI13" s="9"/>
+      <c r="AJ13" s="9"/>
+      <c r="AK13" s="9"/>
+      <c r="AL13" s="9"/>
+      <c r="AM13" s="9"/>
+      <c r="AN13" s="9"/>
+      <c r="AO13" s="9"/>
+      <c r="AP13" s="9"/>
+      <c r="AQ13" s="9"/>
+      <c r="AR13" s="9"/>
+      <c r="AS13" s="9"/>
+      <c r="AT13" s="9"/>
+      <c r="AU13" s="9"/>
+      <c r="AV13" s="9"/>
+      <c r="AW13" s="9"/>
+      <c r="AX13" s="9"/>
+      <c r="AY13" s="9"/>
+      <c r="AZ13" s="9"/>
+      <c r="BA13" s="9"/>
+      <c r="BB13" s="9"/>
+      <c r="BC13" s="9"/>
+      <c r="BD13" s="9"/>
+      <c r="BE13" s="9"/>
+      <c r="BF13" s="9"/>
+      <c r="BG13" s="9"/>
+      <c r="BH13" s="9"/>
+      <c r="BI13" s="9"/>
+      <c r="BJ13" s="9"/>
+      <c r="BK13" s="9"/>
+      <c r="BL13" s="9"/>
+      <c r="BM13" s="9"/>
+      <c r="BN13" s="9"/>
+      <c r="BO13" s="9"/>
+    </row>
+    <row r="14" spans="1:73" x14ac:dyDescent="0.25">
+      <c r="A14" s="20"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="20"/>
+      <c r="L14" s="20"/>
+      <c r="M14" s="20"/>
+      <c r="N14" s="20"/>
+      <c r="O14" s="20"/>
+      <c r="P14" s="20"/>
+      <c r="Q14" s="20"/>
+      <c r="R14" s="20"/>
+      <c r="S14" s="20"/>
+      <c r="T14" s="20"/>
+      <c r="U14" s="20"/>
+      <c r="V14" s="20"/>
+      <c r="W14" s="20"/>
+      <c r="X14" s="20"/>
+      <c r="Y14" s="20"/>
+      <c r="Z14" s="20"/>
+      <c r="AA14" s="20"/>
+      <c r="AB14" s="20"/>
+      <c r="AC14" s="20"/>
+      <c r="AD14" s="20"/>
+      <c r="AE14" s="20"/>
+      <c r="AF14" s="20"/>
+      <c r="AG14" s="20"/>
+      <c r="AH14" s="20"/>
+      <c r="AI14" s="20"/>
+      <c r="AJ14" s="20"/>
+      <c r="AK14" s="20"/>
+      <c r="AL14" s="20"/>
+      <c r="AM14" s="20"/>
+      <c r="AN14" s="20"/>
+      <c r="AO14" s="20"/>
+      <c r="AP14" s="20"/>
+      <c r="AQ14" s="20"/>
+      <c r="AR14" s="20"/>
+      <c r="AS14" s="20"/>
+      <c r="AT14" s="20"/>
+      <c r="AU14" s="20"/>
+      <c r="AV14" s="20"/>
+      <c r="AW14" s="20"/>
+      <c r="AX14" s="20"/>
+      <c r="AY14" s="20"/>
+      <c r="AZ14" s="20"/>
+      <c r="BA14" s="20"/>
+      <c r="BB14" s="20"/>
+      <c r="BC14" s="20"/>
+      <c r="BD14" s="20"/>
+      <c r="BE14" s="20"/>
+      <c r="BF14" s="20"/>
+      <c r="BG14" s="20"/>
+      <c r="BH14" s="20"/>
+      <c r="BI14" s="20"/>
+      <c r="BJ14" s="20"/>
+      <c r="BK14" s="20"/>
+      <c r="BL14" s="20"/>
+      <c r="BM14" s="20"/>
+      <c r="BN14" s="20"/>
+      <c r="BO14" s="20"/>
+    </row>
+    <row r="15" spans="1:73" x14ac:dyDescent="0.25">
+      <c r="A15" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" t="s">
+      <c r="B15" s="22"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
-      <c r="M15" s="10"/>
-      <c r="N15" s="10"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="13"/>
       <c r="O15" s="11"/>
       <c r="P15" s="11"/>
       <c r="Q15" s="11"/>
       <c r="R15" s="11"/>
-      <c r="S15" s="13"/>
-      <c r="T15" s="13"/>
-      <c r="U15" s="13"/>
-      <c r="V15" s="13"/>
-      <c r="W15" s="13"/>
-      <c r="X15" s="13"/>
+      <c r="S15" s="11"/>
+      <c r="T15" s="11"/>
+      <c r="U15" s="11"/>
+      <c r="V15" s="11"/>
+      <c r="W15" s="11"/>
+      <c r="X15" s="11"/>
       <c r="Y15" s="11"/>
-      <c r="Z15" s="11"/>
-      <c r="AA15" s="11"/>
-      <c r="AB15" s="11"/>
-      <c r="AC15" s="11"/>
-      <c r="AD15" s="11"/>
-      <c r="AE15" s="11"/>
+      <c r="Z15" s="14"/>
+      <c r="AA15" s="14"/>
+      <c r="AB15" s="14"/>
+      <c r="AC15" s="14"/>
+      <c r="AD15" s="14"/>
+      <c r="AE15" s="14"/>
       <c r="AF15" s="11"/>
       <c r="AG15" s="11"/>
       <c r="AH15" s="11"/>
@@ -1333,19 +1994,535 @@
       <c r="BC15" s="11"/>
       <c r="BD15" s="11"/>
       <c r="BE15" s="11"/>
-      <c r="BF15" s="11"/>
-      <c r="BG15" s="11"/>
-      <c r="BH15" s="11"/>
-      <c r="BI15" s="11"/>
-      <c r="BJ15" s="11"/>
-      <c r="BK15" s="11"/>
-      <c r="BL15" s="11"/>
-      <c r="BM15" s="11"/>
-      <c r="BN15" s="11"/>
-      <c r="BO15" s="11"/>
+      <c r="BF15" s="19"/>
+      <c r="BG15" s="19"/>
+      <c r="BH15" s="19"/>
+      <c r="BI15" s="19"/>
+      <c r="BJ15" s="19"/>
+      <c r="BK15" s="19"/>
+      <c r="BL15" s="19"/>
+      <c r="BM15" s="19"/>
+      <c r="BN15" s="19"/>
+      <c r="BO15" s="19"/>
+    </row>
+    <row r="16" spans="1:73" x14ac:dyDescent="0.25">
+      <c r="A16" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="21"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="O16" s="15"/>
+      <c r="P16" s="15"/>
+      <c r="Q16" s="15"/>
+      <c r="R16" s="15"/>
+      <c r="S16" s="15"/>
+      <c r="T16" s="15"/>
+      <c r="U16" s="15"/>
+      <c r="V16" s="15"/>
+      <c r="W16" s="15"/>
+      <c r="X16" s="15"/>
+      <c r="Y16" s="15"/>
+      <c r="Z16" s="16"/>
+      <c r="AA16" s="16"/>
+      <c r="AB16" s="16"/>
+      <c r="AC16" s="16"/>
+      <c r="AD16" s="16"/>
+      <c r="AE16" s="16"/>
+      <c r="AF16" s="15"/>
+      <c r="AG16" s="15"/>
+      <c r="AH16" s="15"/>
+      <c r="AI16" s="15"/>
+      <c r="AJ16" s="15"/>
+      <c r="AK16" s="15"/>
+      <c r="AL16" s="15"/>
+      <c r="AM16" s="15"/>
+      <c r="AN16" s="15"/>
+      <c r="AO16" s="15"/>
+      <c r="AP16" s="15"/>
+      <c r="AQ16" s="15"/>
+      <c r="AR16" s="15"/>
+      <c r="AS16" s="15"/>
+      <c r="AT16" s="15"/>
+      <c r="AU16" s="15"/>
+      <c r="AV16" s="15"/>
+      <c r="AW16" s="15"/>
+      <c r="AX16" s="15"/>
+      <c r="AY16" s="15"/>
+      <c r="AZ16" s="15"/>
+      <c r="BA16" s="15"/>
+      <c r="BB16" s="15"/>
+      <c r="BC16" s="15"/>
+      <c r="BD16" s="15"/>
+      <c r="BE16" s="15"/>
+      <c r="BF16" s="17"/>
+      <c r="BG16" s="17"/>
+      <c r="BH16" s="17"/>
+      <c r="BI16" s="17"/>
+      <c r="BJ16" s="17"/>
+      <c r="BK16" s="17"/>
+      <c r="BL16" s="17"/>
+      <c r="BM16" s="17"/>
+      <c r="BN16" s="17"/>
+      <c r="BO16" s="17"/>
+    </row>
+    <row r="17" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="A17" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="20"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="O17" s="7"/>
+      <c r="P17" s="7"/>
+    </row>
+    <row r="18" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="A18" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="20"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q18" s="7"/>
+      <c r="R18" s="7"/>
+      <c r="S18" s="7"/>
+    </row>
+    <row r="19" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="A19" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="20"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="T19" s="7"/>
+      <c r="U19" s="7"/>
+      <c r="V19" s="7"/>
+    </row>
+    <row r="20" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="A20" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="20"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="W20" s="7"/>
+      <c r="X20" s="7"/>
+      <c r="Y20" s="7"/>
+    </row>
+    <row r="21" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="A21" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="20"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="AF21" s="7"/>
+      <c r="AG21" s="7"/>
+      <c r="AH21" s="7"/>
+      <c r="AI21" s="7"/>
+      <c r="AJ21" s="7"/>
+      <c r="AK21" s="7"/>
+      <c r="AL21" s="7"/>
+    </row>
+    <row r="22" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="A22" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="20"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="AM22" s="7"/>
+      <c r="AN22" s="7"/>
+      <c r="AO22" s="7"/>
+      <c r="AP22" s="7"/>
+      <c r="AQ22" s="7"/>
+      <c r="AR22" s="7"/>
+      <c r="AS22" s="7"/>
+    </row>
+    <row r="23" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="A23" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="20"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="AM23" s="7"/>
+      <c r="AN23" s="7"/>
+      <c r="AO23" s="7"/>
+      <c r="AP23" s="7"/>
+      <c r="AQ23" s="7"/>
+      <c r="AR23" s="7"/>
+      <c r="AS23" s="7"/>
+    </row>
+    <row r="24" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="A24" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="20"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="AT24" s="7"/>
+      <c r="AU24" s="7"/>
+      <c r="AV24" s="7"/>
+      <c r="AW24" s="7"/>
+      <c r="AX24" s="7"/>
+      <c r="AY24" s="7"/>
+      <c r="AZ24" s="7"/>
+    </row>
+    <row r="25" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="A25" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="20"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="BA25" s="7"/>
+      <c r="BB25" s="7"/>
+      <c r="BC25" s="7"/>
+    </row>
+    <row r="26" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="A26" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" s="20"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="BD26" s="7"/>
+      <c r="BE26" s="7"/>
+    </row>
+    <row r="27" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="A27" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" s="20"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="N27" s="17"/>
+      <c r="BD27" s="17"/>
+      <c r="BE27" s="17"/>
+      <c r="BF27" s="17"/>
+      <c r="BG27" s="17"/>
+      <c r="BH27" s="17"/>
+      <c r="BI27" s="17"/>
+      <c r="BJ27" s="17"/>
+      <c r="BK27" s="17"/>
+    </row>
+    <row r="28" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="A28" s="20"/>
+      <c r="B28" s="20"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="9"/>
+    </row>
+    <row r="29" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="A29" s="20"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="9"/>
+    </row>
+    <row r="30" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="A30" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30" s="21"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q30" s="17"/>
+      <c r="R30" s="17"/>
+      <c r="S30" s="17"/>
+      <c r="T30" s="15"/>
+      <c r="U30" s="15"/>
+      <c r="V30" s="15"/>
+      <c r="W30" s="15"/>
+      <c r="X30" s="15"/>
+      <c r="Y30" s="15"/>
+      <c r="Z30" s="16"/>
+      <c r="AA30" s="16"/>
+      <c r="AB30" s="16"/>
+      <c r="AC30" s="16"/>
+      <c r="AD30" s="16"/>
+      <c r="AE30" s="16"/>
+      <c r="AF30" s="15"/>
+      <c r="AG30" s="15"/>
+      <c r="AH30" s="15"/>
+      <c r="AI30" s="15"/>
+      <c r="AJ30" s="15"/>
+      <c r="AK30" s="15"/>
+      <c r="AL30" s="15"/>
+      <c r="AM30" s="15"/>
+      <c r="AN30" s="15"/>
+      <c r="AO30" s="15"/>
+      <c r="AP30" s="15"/>
+      <c r="AQ30" s="15"/>
+      <c r="AR30" s="15"/>
+      <c r="AS30" s="15"/>
+      <c r="AT30" s="15"/>
+      <c r="AU30" s="15"/>
+      <c r="AV30" s="15"/>
+      <c r="AW30" s="15"/>
+      <c r="AX30" s="15"/>
+      <c r="AY30" s="15"/>
+      <c r="AZ30" s="15"/>
+      <c r="BA30" s="15"/>
+      <c r="BB30" s="15"/>
+      <c r="BC30" s="15"/>
+      <c r="BD30" s="15"/>
+      <c r="BE30" s="15"/>
+      <c r="BF30" s="15"/>
+      <c r="BG30" s="15"/>
+      <c r="BH30" s="15"/>
+      <c r="BI30" s="15"/>
+      <c r="BJ30" s="15"/>
+      <c r="BK30" s="15"/>
+      <c r="BL30" s="15"/>
+      <c r="BM30" s="15"/>
+      <c r="BN30" s="15"/>
+      <c r="BO30" s="17"/>
+    </row>
+    <row r="31" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="A31" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31" s="20"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="T31" s="7"/>
+      <c r="U31" s="7"/>
+    </row>
+    <row r="32" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="A32" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="B32" s="20"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="V32" s="7"/>
+      <c r="W32" s="7"/>
+      <c r="X32" s="7"/>
+    </row>
+    <row r="33" spans="1:73" x14ac:dyDescent="0.25">
+      <c r="A33" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B33" s="20"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="X33" s="7"/>
+      <c r="Y33" s="7"/>
+      <c r="Z33" s="17"/>
+    </row>
+    <row r="34" spans="1:73" x14ac:dyDescent="0.25">
+      <c r="A34" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34" s="20"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="AF34" s="7"/>
+      <c r="AG34" s="7"/>
+      <c r="AH34" s="7"/>
+      <c r="AI34" s="7"/>
+    </row>
+    <row r="35" spans="1:73" x14ac:dyDescent="0.25">
+      <c r="A35" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" s="20"/>
+      <c r="C35" s="20"/>
+      <c r="D35" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="AJ35" s="7"/>
+      <c r="AK35" s="7"/>
+      <c r="AL35" s="7"/>
+      <c r="AM35" s="7"/>
+      <c r="AN35" s="7"/>
+      <c r="AO35" s="7"/>
+      <c r="AP35" s="7"/>
+    </row>
+    <row r="36" spans="1:73" x14ac:dyDescent="0.25">
+      <c r="A36" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36" s="20"/>
+      <c r="C36" s="20"/>
+      <c r="D36" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="AP36" s="7"/>
+      <c r="AQ36" s="7"/>
+      <c r="AR36" s="7"/>
+      <c r="AS36" s="7"/>
+      <c r="AT36" s="7"/>
+      <c r="AU36" s="7"/>
+      <c r="AV36" s="7"/>
+    </row>
+    <row r="37" spans="1:73" x14ac:dyDescent="0.25">
+      <c r="A37" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37" s="20"/>
+      <c r="C37" s="20"/>
+      <c r="D37" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="AQ37" s="7"/>
+      <c r="AR37" s="7"/>
+      <c r="AS37" s="7"/>
+      <c r="AT37" s="7"/>
+      <c r="AU37" s="7"/>
+      <c r="AV37" s="7"/>
+      <c r="AW37" s="7"/>
+    </row>
+    <row r="38" spans="1:73" x14ac:dyDescent="0.25">
+      <c r="A38" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B38" s="20"/>
+      <c r="C38" s="20"/>
+      <c r="D38" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="AW38" s="7"/>
+      <c r="AX38" s="7"/>
+      <c r="AY38" s="7"/>
+      <c r="AZ38" s="7"/>
+      <c r="BA38" s="7"/>
+      <c r="BB38" s="7"/>
+      <c r="BC38" s="7"/>
+    </row>
+    <row r="39" spans="1:73" x14ac:dyDescent="0.25">
+      <c r="A39" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39" s="20"/>
+      <c r="C39" s="20"/>
+      <c r="D39" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="BC39" s="7"/>
+      <c r="BD39" s="7"/>
+      <c r="BE39" s="7"/>
+    </row>
+    <row r="40" spans="1:73" x14ac:dyDescent="0.25">
+      <c r="A40" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B40" s="20"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="BF40" s="7"/>
+      <c r="BG40" s="7"/>
+      <c r="BH40" s="17"/>
+    </row>
+    <row r="41" spans="1:73" x14ac:dyDescent="0.25">
+      <c r="A41" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B41" s="20"/>
+      <c r="C41" s="20"/>
+      <c r="D41" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="BH41" s="7"/>
+      <c r="BI41" s="7"/>
+      <c r="BJ41" s="7"/>
+      <c r="BK41" s="7"/>
+      <c r="BL41" s="7"/>
+      <c r="BM41" s="7"/>
+      <c r="BN41" s="7"/>
+    </row>
+    <row r="43" spans="1:73" x14ac:dyDescent="0.25">
+      <c r="A43" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="B43" s="22"/>
+      <c r="C43" s="22"/>
+      <c r="D43" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="BO43" s="15"/>
+      <c r="BP43" s="15"/>
+      <c r="BQ43" s="15"/>
+      <c r="BR43" s="15"/>
+      <c r="BS43" s="15"/>
+      <c r="BT43" s="15"/>
+      <c r="BU43" s="15"/>
+    </row>
+    <row r="44" spans="1:73" x14ac:dyDescent="0.25">
+      <c r="A44" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="B44" s="20"/>
+      <c r="C44" s="20"/>
+      <c r="D44" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="BO44" s="7"/>
+      <c r="BP44" s="7"/>
+      <c r="BQ44" s="7"/>
+      <c r="BR44" s="7"/>
+      <c r="BS44" s="7"/>
+      <c r="BT44" s="7"/>
+      <c r="BU44" s="7"/>
+    </row>
+    <row r="45" spans="1:73" x14ac:dyDescent="0.25">
+      <c r="A45" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="B45" s="20"/>
+      <c r="C45" s="20"/>
+      <c r="D45" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="BO45" s="7"/>
+      <c r="BP45" s="7"/>
+      <c r="BQ45" s="7"/>
+      <c r="BR45" s="7"/>
+      <c r="BS45" s="7"/>
+      <c r="BT45" s="7"/>
+      <c r="BU45" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="42">
+    <mergeCell ref="A43:C43"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="A45:C45"/>
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="A5:C5"/>
     <mergeCell ref="A3:C3"/>
@@ -1359,116 +2536,34 @@
     <mergeCell ref="A9:C9"/>
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A40:C40"/>
+    <mergeCell ref="A41:C41"/>
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="A37:C37"/>
+    <mergeCell ref="A38:C38"/>
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="A28:C28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>